<commit_message>
Atualização - Diminuir código
Ajuste na planilha e diminuição no código de launcher
</commit_message>
<xml_diff>
--- a/data/NFTS_db.xlsx
+++ b/data/NFTS_db.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f99ddde0a66b2902/Documentos/GitHub/Automacao-emissao-NFTS/Dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f99ddde0a66b2902/Documentos/GitHub/Automacao-emissao-NFTS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="11_985998E503861325E190350CDFED3F8BA590ECD8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E99DAA4-C4DA-4617-B241-E635B6DD5210}"/>
+  <xr:revisionPtr revIDLastSave="472" documentId="11_985998E503861325E190350CDFED3F8BA590ECD8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A8B007-5C73-4EB5-97FB-2C07D89B0AD8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Dados_NF" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dados_NF!$A$1:$V$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dados_NF!$A$1:$P$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Numero_NF</t>
   </si>
@@ -84,9 +84,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>2,59</t>
-  </si>
-  <si>
     <t>SP</t>
   </si>
   <si>
@@ -138,18 +135,6 @@
     <t>RJ</t>
   </si>
   <si>
-    <t>03030-713</t>
-  </si>
-  <si>
-    <t>01010-711</t>
-  </si>
-  <si>
-    <t>02020-712</t>
-  </si>
-  <si>
-    <t>04040-714</t>
-  </si>
-  <si>
     <t>Esse serviço é ficticio. (Limpeza)</t>
   </si>
   <si>
@@ -162,21 +147,6 @@
     <t>ID_pagamento</t>
   </si>
   <si>
-    <t>1.758,5</t>
-  </si>
-  <si>
-    <t>3.700,7</t>
-  </si>
-  <si>
-    <t>19.050,57</t>
-  </si>
-  <si>
-    <t>200,25</t>
-  </si>
-  <si>
-    <t>755,25</t>
-  </si>
-  <si>
     <t>Razao_Social</t>
   </si>
   <si>
@@ -192,51 +162,38 @@
     <t>Nexus Dynamics Group</t>
   </si>
   <si>
-    <t>10.875,85</t>
-  </si>
-  <si>
-    <t>Tipo_Endereco</t>
-  </si>
-  <si>
-    <t>Endereco</t>
-  </si>
-  <si>
-    <t>Numero</t>
-  </si>
-  <si>
-    <t>Complemento</t>
-  </si>
-  <si>
-    <t>Bairro</t>
-  </si>
-  <si>
-    <t>Rua</t>
-  </si>
-  <si>
-    <t>Mafranz</t>
-  </si>
-  <si>
-    <t>Rua do parque</t>
-  </si>
-  <si>
-    <t>Jardim prainha</t>
-  </si>
-  <si>
-    <t>255,2</t>
-  </si>
-  <si>
-    <t>1855,2</t>
+    <t>17.02</t>
+  </si>
+  <si>
+    <t>17.03</t>
+  </si>
+  <si>
+    <t>17.04</t>
+  </si>
+  <si>
+    <t>01.02</t>
+  </si>
+  <si>
+    <t>01.010-101</t>
+  </si>
+  <si>
+    <t>02.020-712</t>
+  </si>
+  <si>
+    <t>03.030-713</t>
+  </si>
+  <si>
+    <t>04.040-714</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -380,9 +337,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -424,19 +381,25 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -776,39 +739,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="13">
         <v>12345678</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -827,10 +790,10 @@
   <sheetPr codeName="Sheet2">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29:K29"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,22 +804,21 @@
     <col min="4" max="4" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="7" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="18" width="18" style="7" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="33.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.85546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -873,7 +835,7 @@
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -886,297 +848,231 @@
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>146.15100000000001</v>
+    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>111111</v>
       </c>
       <c r="B2" s="3">
         <v>2577</v>
       </c>
-      <c r="C2" s="16">
-        <v>45447</v>
+      <c r="C2" s="20">
+        <v>45391</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>61</v>
+      <c r="E2" s="19">
+        <v>1758.5</v>
+      </c>
+      <c r="F2" s="18">
+        <v>255.2</v>
       </c>
       <c r="G2" s="3">
-        <v>321</v>
-      </c>
-      <c r="H2" s="1">
-        <v>17.010000000000002</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>15</v>
+        <v>1872</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.5</v>
       </c>
       <c r="J2" s="2">
         <v>2</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="3">
-        <v>1245678</v>
-      </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>146.15199999999999</v>
+        <v>23</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>222222</v>
       </c>
       <c r="B3" s="3">
         <v>179</v>
       </c>
-      <c r="C3" s="16">
-        <v>45447</v>
+      <c r="C3" s="20">
+        <v>45391</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>44</v>
+      <c r="E3" s="19">
+        <v>3700.7</v>
+      </c>
+      <c r="F3" s="18">
+        <v>200.25</v>
       </c>
       <c r="G3" s="3">
-        <v>22333</v>
-      </c>
-      <c r="H3" s="1">
-        <v>17.02</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>15</v>
+        <v>1538</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2.59</v>
       </c>
       <c r="J3" s="2">
         <v>2</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="N3" s="3" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="P3" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="V3" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>146.15299999999999</v>
+        <v>46</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>333333</v>
       </c>
       <c r="B4" s="3">
         <v>256</v>
       </c>
-      <c r="C4" s="16">
-        <v>45447</v>
+      <c r="C4" s="20">
+        <v>45391</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>45</v>
+      <c r="E4" s="19">
+        <v>10875.85</v>
+      </c>
+      <c r="F4" s="18">
+        <v>755.25</v>
       </c>
       <c r="G4" s="3">
-        <v>22333</v>
-      </c>
-      <c r="H4" s="1">
-        <v>17.03</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>15</v>
+        <v>1503</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2.59</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="3">
-        <v>1245678</v>
-      </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="U4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="V4" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>146.154</v>
+    </row>
+    <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>444444</v>
       </c>
       <c r="B5" s="3">
         <v>256183</v>
       </c>
-      <c r="C5" s="16">
-        <v>45447</v>
+      <c r="C5" s="20">
+        <v>45391</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="19">
+        <v>19050.57</v>
+      </c>
+      <c r="F5" s="18">
+        <v>1855.2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1481</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="3">
-        <v>22329</v>
-      </c>
-      <c r="H5" s="1">
-        <v>17.04</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>15</v>
+      <c r="I5" s="3">
+        <v>2.59</v>
       </c>
       <c r="J5" s="2">
         <v>2</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="N5" s="3" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="P5" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="V5" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="1"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1186,20 +1082,14 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-    </row>
-    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="3"/>
       <c r="E7" s="1"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="1"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1209,20 +1099,14 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-    </row>
-    <row r="8" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="1"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1232,20 +1116,14 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-    </row>
-    <row r="9" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="3"/>
       <c r="E9" s="1"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1255,37 +1133,34 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F10" s="18"/>
-      <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F11" s="18"/>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F12" s="18"/>
-      <c r="G12" s="15"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F10" s="17"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F11" s="17"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F12" s="17"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F13" s="17"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H14" s="14"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H16" s="14"/>
     </row>
   </sheetData>

</xml_diff>